<commit_message>
Updated wrap-up form links
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-scRNAseq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0E69BA-4DC1-1D47-9DE1-1E7E152485ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5BA9D0-3964-E241-B54A-E401CEA47DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="48540" yWindow="7980" windowWidth="29860" windowHeight="21100" xr2:uid="{4D37F018-551B-CF4D-85BF-2DD74B664EBF}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
   <si>
     <t>date</t>
   </si>
@@ -197,21 +197,6 @@
     <t>link_form</t>
   </si>
   <si>
-    <t>https://forms.gle/gATSp2VCSBXCMDaU9</t>
-  </si>
-  <si>
-    <t>https://forms.gle/i9Vic1o3ZB83vSiH9</t>
-  </si>
-  <si>
-    <t>https://forms.gle/B9Tt7QqpBJsBmjRV6</t>
-  </si>
-  <si>
-    <t>https://forms.gle/iZumacPY1iyscZPHA</t>
-  </si>
-  <si>
-    <t>https://forms.gle/D66Y3ShaamWeJZm87</t>
-  </si>
-  <si>
     <t>Lecture: Data normalization</t>
   </si>
   <si>
@@ -285,6 +270,18 @@
   </si>
   <si>
     <t>AB, YL</t>
+  </si>
+  <si>
+    <t>https://forms.gle/Bxz2QtqWa6ku2YjL6</t>
+  </si>
+  <si>
+    <t>https://forms.gle/vf2Bsb56z3avQaiJ6</t>
+  </si>
+  <si>
+    <t>https://forms.gle/dqkXKABN7B2FS81G8</t>
+  </si>
+  <si>
+    <t>https://forms.gle/MLyMdWiMfKfLpFZv7</t>
   </si>
 </sst>
 </file>
@@ -660,7 +657,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,10 +715,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3">
         <v>0.375</v>
@@ -730,19 +727,19 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -753,13 +750,13 @@
         <v>0.4375</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -816,7 +813,7 @@
         <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H7" t="s">
         <v>33</v>
@@ -837,10 +834,10 @@
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -862,7 +859,7 @@
         <v>0.6875</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
@@ -885,12 +882,12 @@
         <v>12</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C12" s="3">
         <v>0.375</v>
@@ -899,10 +896,10 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H12" t="s">
         <v>35</v>
@@ -931,13 +928,13 @@
         <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="K14" s="1"/>
     </row>
@@ -963,7 +960,7 @@
         <v>22</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H16" t="s">
         <v>36</v>
@@ -981,13 +978,13 @@
         <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I17" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="K17" s="1"/>
     </row>
@@ -1033,7 +1030,7 @@
         <v>12</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1044,12 +1041,12 @@
         <v>0.875</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C22" s="3">
         <v>0.375</v>
@@ -1064,10 +1061,10 @@
         <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I22" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="K22" s="1"/>
     </row>
@@ -1120,10 +1117,10 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E26" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F26" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H26" t="s">
         <v>39</v>
@@ -1137,10 +1134,10 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="E27" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F27" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H27" t="s">
         <v>40</v>
@@ -1169,13 +1166,13 @@
         <v>26</v>
       </c>
       <c r="F29" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G29" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I29" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1192,12 +1189,12 @@
         <v>12</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C31" s="3">
         <v>0.375</v>
@@ -1209,7 +1206,7 @@
         <v>27</v>
       </c>
       <c r="F31" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H31" t="s">
         <v>41</v>
@@ -1238,13 +1235,13 @@
         <v>28</v>
       </c>
       <c r="F33" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G33" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I33" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -1270,7 +1267,7 @@
         <v>29</v>
       </c>
       <c r="F35" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H35" t="s">
         <v>42</v>
@@ -1287,13 +1284,13 @@
         <v>30</v>
       </c>
       <c r="F36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G36" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I36" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -1321,12 +1318,12 @@
         <v>12</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C39" s="3">
         <v>0.375</v>
@@ -1335,13 +1332,13 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="E39" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F39" t="s">
         <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -1352,13 +1349,13 @@
         <v>0.5</v>
       </c>
       <c r="E40" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F40" t="s">
         <v>12</v>
       </c>
       <c r="G40" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -1388,19 +1385,15 @@
       <c r="H42" t="s">
         <v>43</v>
       </c>
-      <c r="J42" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="J42" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" display="https://nbisweden.github.io/workshop-scRNAseq/lectures/course_intro_Asa_Bjorklund_2023.pdf" xr:uid="{4DD82CAF-94BD-B14A-90E7-31931BE24C2F}"/>
-    <hyperlink ref="J42" r:id="rId2" xr:uid="{A47D8860-97C8-C74F-9F24-40DBC0A812B9}"/>
-    <hyperlink ref="J38" r:id="rId3" xr:uid="{5F7630BD-131A-7947-B9CF-E27EB34835ED}"/>
-    <hyperlink ref="J30" r:id="rId4" xr:uid="{263745C2-CFBD-1542-BD8B-033F5C1425FF}"/>
-    <hyperlink ref="J20" r:id="rId5" xr:uid="{88A1381F-8CCC-7941-996A-13E6C41216A9}"/>
-    <hyperlink ref="J11" r:id="rId6" xr:uid="{4172D9DB-A0D4-4E45-A075-48707F36AF9C}"/>
-    <hyperlink ref="L2" r:id="rId7" xr:uid="{3C7901EF-0BB8-A14F-9DFF-E5982A422C2F}"/>
+    <hyperlink ref="J30" r:id="rId2" xr:uid="{263745C2-CFBD-1542-BD8B-033F5C1425FF}"/>
+    <hyperlink ref="J20" r:id="rId3" xr:uid="{88A1381F-8CCC-7941-996A-13E6C41216A9}"/>
+    <hyperlink ref="J11" r:id="rId4" xr:uid="{4172D9DB-A0D4-4E45-A075-48707F36AF9C}"/>
+    <hyperlink ref="L2" r:id="rId5" xr:uid="{3C7901EF-0BB8-A14F-9DFF-E5982A422C2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Paulo to trajectory
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-scRNAseq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5BA9D0-3964-E241-B54A-E401CEA47DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB41CE2-6982-2949-A222-3FD8E40395AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48540" yWindow="7980" windowWidth="29860" windowHeight="21100" xr2:uid="{4D37F018-551B-CF4D-85BF-2DD74B664EBF}"/>
+    <workbookView xWindow="46940" yWindow="7980" windowWidth="29860" windowHeight="21100" xr2:uid="{4D37F018-551B-CF4D-85BF-2DD74B664EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
   <si>
     <t>date</t>
   </si>
@@ -77,9 +77,6 @@
     <t>topic</t>
   </si>
   <si>
-    <t>teacher</t>
-  </si>
-  <si>
     <t>assistant</t>
   </si>
   <si>
@@ -282,6 +279,12 @@
   </si>
   <si>
     <t>https://forms.gle/MLyMdWiMfKfLpFZv7</t>
+  </si>
+  <si>
+    <t>instructor</t>
+  </si>
+  <si>
+    <t>Paulo Czarnewski</t>
   </si>
 </sst>
 </file>
@@ -657,7 +660,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,33 +695,33 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="3">
         <v>0.375</v>
@@ -727,19 +730,19 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -750,13 +753,13 @@
         <v>0.4375</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -768,7 +771,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -779,13 +782,13 @@
         <v>0.5</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -796,7 +799,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -807,16 +810,16 @@
         <v>0.5625</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -828,16 +831,16 @@
         <v>0.625</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -848,7 +851,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -859,13 +862,13 @@
         <v>0.6875</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -876,18 +879,18 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="3">
         <v>0.375</v>
@@ -896,13 +899,13 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K12" s="1"/>
     </row>
@@ -914,7 +917,7 @@
         <v>0.4375</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -925,16 +928,16 @@
         <v>0.5</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K14" s="1"/>
     </row>
@@ -946,7 +949,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -957,13 +960,13 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K16" s="1"/>
     </row>
@@ -975,16 +978,16 @@
         <v>0.625</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K17" s="1"/>
     </row>
@@ -996,7 +999,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1007,13 +1010,13 @@
         <v>0.6875</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1024,13 +1027,13 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1041,12 +1044,12 @@
         <v>0.875</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="3">
         <v>0.375</v>
@@ -1055,16 +1058,16 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K22" s="1"/>
     </row>
@@ -1076,7 +1079,7 @@
         <v>0.4375</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1087,13 +1090,13 @@
         <v>0.5</v>
       </c>
       <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s">
         <v>24</v>
       </c>
-      <c r="F24" t="s">
-        <v>25</v>
-      </c>
       <c r="H24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K24" s="1"/>
     </row>
@@ -1105,7 +1108,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K25" s="1"/>
     </row>
@@ -1117,13 +1120,13 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -1134,13 +1137,13 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="E27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K27" s="1"/>
     </row>
@@ -1152,7 +1155,7 @@
         <v>0.625</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1163,16 +1166,16 @@
         <v>0.6875</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1183,18 +1186,18 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" s="3">
         <v>0.375</v>
@@ -1203,13 +1206,13 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K31" s="1"/>
     </row>
@@ -1221,7 +1224,7 @@
         <v>0.4375</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -1232,16 +1235,16 @@
         <v>0.5</v>
       </c>
       <c r="E33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -1252,7 +1255,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K34" s="1"/>
     </row>
@@ -1264,13 +1267,13 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F35" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="H35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -1281,16 +1284,16 @@
         <v>0.625</v>
       </c>
       <c r="E36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F36" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="G36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -1301,7 +1304,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="E37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -1312,18 +1315,18 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" s="3">
         <v>0.375</v>
@@ -1332,13 +1335,13 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="E39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -1349,13 +1352,13 @@
         <v>0.5</v>
       </c>
       <c r="E40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -1366,7 +1369,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -1377,13 +1380,13 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J42" s="1"/>
     </row>

</xml_diff>

<commit_message>
schedule updates and lecture slides
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asabjor/courses/course_git/workshop-scRNAseq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED58727-7CFE-6549-B479-6CC28F710760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513620C3-9F00-094F-8D02-9D40BEDC754C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8080" yWindow="860" windowWidth="35100" windowHeight="24660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9780" yWindow="500" windowWidth="28620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -231,18 +231,6 @@
     <t>Jennifer Fransson</t>
   </si>
   <si>
-    <t>https://forms.gle/qdnNeb17Jk6FpW9b7</t>
-  </si>
-  <si>
-    <t>https://forms.gle/WLCE7ZD1Wpj6qUUq9</t>
-  </si>
-  <si>
-    <t>https://forms.gle/bhvJfG4xY1DL1vhEA</t>
-  </si>
-  <si>
-    <t>https://forms.gle/TqH9yS9meS9UqpFR9</t>
-  </si>
-  <si>
     <t>Fariba Roshanzamir</t>
   </si>
   <si>
@@ -250,6 +238,18 @@
   </si>
   <si>
     <t>Lecture: scRNAseq methods and NGI</t>
+  </si>
+  <si>
+    <t>https://forms.gle/CgiN3CkoCKyu6rWy7</t>
+  </si>
+  <si>
+    <t>https://forms.gle/jHfsMjZR5kNcXhfAA</t>
+  </si>
+  <si>
+    <t>https://forms.gle/mfLYo7eK97DpEx819</t>
+  </si>
+  <si>
+    <t>https://forms.gle/VZwkpUbTs4y1DDhv5</t>
   </si>
 </sst>
 </file>
@@ -689,7 +689,7 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -777,7 +777,7 @@
         <v>0.4375</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
@@ -903,7 +903,7 @@
         <v>63</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -949,7 +949,7 @@
         <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="I14" t="s">
         <v>24</v>
@@ -996,7 +996,7 @@
         <v>34</v>
       </c>
       <c r="F17" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="I17" t="s">
         <v>24</v>
@@ -1045,7 +1045,7 @@
         <v>63</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1092,13 +1092,13 @@
         <v>0.5</v>
       </c>
       <c r="E24" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F24" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="H24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K24" s="3"/>
     </row>
@@ -1122,13 +1122,13 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F26" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="H26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -1191,7 +1191,7 @@
         <v>63</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -1208,7 +1208,7 @@
         <v>45</v>
       </c>
       <c r="F31" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H31" t="s">
         <v>46</v>
@@ -1237,7 +1237,7 @@
         <v>47</v>
       </c>
       <c r="F33" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I33" t="s">
         <v>24</v>
@@ -1283,7 +1283,7 @@
         <v>51</v>
       </c>
       <c r="F36" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="I36" t="s">
         <v>24</v>
@@ -1317,7 +1317,7 @@
         <v>55</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -1328,7 +1328,7 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="E39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F39" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Update schedule and render
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asabjor/courses/course_git/workshop-scRNAseq/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenfra/NBISCourses/scRNAseq/workshop-scRNAseq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513620C3-9F00-094F-8D02-9D40BEDC754C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B83F03-9982-4E42-9BA4-6DCFFBAEF148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9780" yWindow="500" windowWidth="28620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$L$41</definedName>
+    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$L$42</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
   <si>
     <t>date</t>
   </si>
@@ -390,9 +390,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -430,7 +430,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -536,7 +536,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -678,7 +678,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -686,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1089,7 +1089,7 @@
         <v>0.4375</v>
       </c>
       <c r="D24" s="2">
-        <v>0.5</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="E24" t="s">
         <v>41</v>
@@ -1104,263 +1104,267 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C25" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D25" s="2">
         <v>0.5</v>
       </c>
-      <c r="D25" s="2">
-        <v>0.54166666666666696</v>
-      </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>43</v>
+      </c>
+      <c r="F25" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" t="s">
+        <v>56</v>
       </c>
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C26" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="2">
         <v>0.54166666666666696</v>
       </c>
-      <c r="D26" s="2">
-        <v>0.58333333333333304</v>
-      </c>
       <c r="E26" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" t="s">
-        <v>39</v>
-      </c>
-      <c r="H26" t="s">
-        <v>40</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C27" s="2">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D27" s="2">
         <v>0.58333333333333304</v>
       </c>
-      <c r="D27" s="2">
-        <v>0.60416666666666696</v>
-      </c>
       <c r="E27" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F27" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="H27" t="s">
-        <v>56</v>
-      </c>
-      <c r="K27" s="3"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C28" s="2">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="D28" s="2">
         <v>0.60416666666666696</v>
       </c>
-      <c r="D28" s="2">
-        <v>0.625</v>
-      </c>
       <c r="E28" t="s">
-        <v>17</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I28" t="s">
+        <v>24</v>
+      </c>
+      <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C29" s="2">
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="D29" s="2">
         <v>0.625</v>
       </c>
-      <c r="D29" s="2">
-        <v>0.6875</v>
-      </c>
       <c r="E29" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" t="s">
-        <v>66</v>
-      </c>
-      <c r="I29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C30" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D30" s="2">
         <v>0.6875</v>
       </c>
-      <c r="D30" s="2">
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C31" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="D31" s="2">
         <v>0.70833333333333304</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>27</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" t="s">
         <v>63</v>
       </c>
-      <c r="J30" s="3" t="s">
+      <c r="J31" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C32" s="2">
         <v>0.375</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D32" s="2">
         <v>0.41666666666666702</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>45</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>67</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H32" t="s">
         <v>46</v>
       </c>
-      <c r="K31" s="3"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C32" s="2">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.4375</v>
-      </c>
-      <c r="E32" t="s">
-        <v>17</v>
-      </c>
+      <c r="K32" s="3"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C33" s="2">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="D33" s="2">
         <v>0.4375</v>
       </c>
-      <c r="D33" s="2">
-        <v>0.5</v>
-      </c>
       <c r="E33" t="s">
-        <v>47</v>
-      </c>
-      <c r="F33" t="s">
-        <v>67</v>
-      </c>
-      <c r="I33" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C34" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D34" s="2">
         <v>0.5</v>
       </c>
-      <c r="D34" s="2">
-        <v>0.54166666666666696</v>
-      </c>
       <c r="E34" t="s">
-        <v>20</v>
-      </c>
-      <c r="K34" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="F34" t="s">
+        <v>67</v>
+      </c>
+      <c r="I34" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C35" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D35" s="2">
         <v>0.54166666666666696</v>
       </c>
-      <c r="D35" s="2">
-        <v>0.58333333333333304</v>
-      </c>
       <c r="E35" t="s">
-        <v>48</v>
-      </c>
-      <c r="F35" t="s">
-        <v>49</v>
-      </c>
-      <c r="H35" t="s">
-        <v>50</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="K35" s="3"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C36" s="2">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D36" s="2">
         <v>0.58333333333333304</v>
       </c>
-      <c r="D36" s="2">
-        <v>0.64583333333333337</v>
-      </c>
       <c r="E36" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I36" t="s">
-        <v>24</v>
+        <v>49</v>
+      </c>
+      <c r="H36" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C37" s="2">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="D37" s="2">
         <v>0.64583333333333337</v>
       </c>
-      <c r="D37" s="2">
-        <v>0.66666666666666663</v>
-      </c>
       <c r="E37" t="s">
-        <v>17</v>
+        <v>51</v>
+      </c>
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C38" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D38" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D38" s="2">
-        <v>0.6875</v>
-      </c>
       <c r="E38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F38" t="s">
-        <v>63</v>
-      </c>
-      <c r="H38" t="s">
-        <v>55</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C39" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D39" s="2">
         <v>0.6875</v>
       </c>
-      <c r="D39" s="2">
-        <v>0.70833333333333304</v>
-      </c>
       <c r="E39" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="F39" t="s">
         <v>63</v>
       </c>
-      <c r="J39" s="3"/>
+      <c r="H39" t="s">
+        <v>55</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>58</v>
-      </c>
       <c r="C40" s="2">
-        <v>0.375</v>
+        <v>0.6875</v>
       </c>
       <c r="D40" s="2">
-        <v>0.39583333333333298</v>
+        <v>0.70833333333333304</v>
       </c>
       <c r="E40" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="F40" t="s">
         <v>63</v>
       </c>
+      <c r="J40" s="3"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>58</v>
+      </c>
       <c r="C41" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D41" s="2">
         <v>0.39583333333333298</v>
       </c>
-      <c r="D41" s="2">
-        <v>0.5</v>
-      </c>
       <c r="E41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F41" t="s">
         <v>63</v>
@@ -1368,55 +1372,69 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C42" s="2">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="D42" s="2">
         <v>0.5</v>
       </c>
-      <c r="D42" s="2">
-        <v>0.54166666666666696</v>
-      </c>
       <c r="E42" t="s">
-        <v>20</v>
+        <v>53</v>
+      </c>
+      <c r="F42" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C43" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D43" s="2">
         <v>0.54166666666666696</v>
       </c>
-      <c r="D43" s="2">
-        <v>0.60416666666666663</v>
-      </c>
       <c r="E43" t="s">
-        <v>53</v>
-      </c>
-      <c r="F43" t="s">
-        <v>63</v>
-      </c>
-      <c r="J43" s="3"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C44" s="2">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D44" s="2">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D44" s="2">
-        <v>0.66666666666666663</v>
-      </c>
       <c r="E44" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F44" t="s">
         <v>63</v>
       </c>
+      <c r="J44" s="3"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C45" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D45" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D45" s="2">
+      <c r="E45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C46" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D46" s="2">
         <v>0.6875</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E46" t="s">
         <v>65</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F46" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add BYOD intro and DM slides
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenfra/NBISCourses/scRNAseq/workshop-scRNAseq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583E30B3-57AB-DF41-A7DC-127382B63003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFADA04-2E23-3B44-B077-F414B0FC4A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9780" yWindow="500" windowWidth="28620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18160" yWindow="3220" windowWidth="28620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="80">
   <si>
     <t>date</t>
   </si>
@@ -259,6 +259,15 @@
   </si>
   <si>
     <t>lectures/gsa.pdf</t>
+  </si>
+  <si>
+    <t>lectures/DataManagement.pdf</t>
+  </si>
+  <si>
+    <t>Intro to Data Management</t>
+  </si>
+  <si>
+    <t>lectures/BYOD_intro.pdf</t>
   </si>
 </sst>
 </file>
@@ -695,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1379,7 +1388,7 @@
         <v>0.375</v>
       </c>
       <c r="D41" s="2">
-        <v>0.39583333333333298</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="E41" t="s">
         <v>52</v>
@@ -1387,56 +1396,59 @@
       <c r="F41" t="s">
         <v>63</v>
       </c>
+      <c r="H41" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C42" s="2">
-        <v>0.39583333333333298</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="D42" s="2">
-        <v>0.5</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="E42" t="s">
-        <v>53</v>
-      </c>
-      <c r="F42" t="s">
-        <v>63</v>
+        <v>78</v>
+      </c>
+      <c r="H42" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C43" s="2">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="D43" s="2">
         <v>0.5</v>
       </c>
-      <c r="D43" s="2">
-        <v>0.54166666666666696</v>
-      </c>
       <c r="E43" t="s">
-        <v>20</v>
+        <v>53</v>
+      </c>
+      <c r="F43" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C44" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D44" s="2">
         <v>0.54166666666666696</v>
       </c>
-      <c r="D44" s="2">
-        <v>0.60416666666666663</v>
-      </c>
       <c r="E44" t="s">
-        <v>53</v>
-      </c>
-      <c r="F44" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="J44" s="3"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C45" s="2">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D45" s="2">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D45" s="2">
-        <v>0.66666666666666663</v>
-      </c>
       <c r="E45" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F45" t="s">
         <v>63</v>
@@ -1444,15 +1456,29 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C46" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D46" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D46" s="2">
+      <c r="E46" t="s">
+        <v>64</v>
+      </c>
+      <c r="F46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C47" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D47" s="2">
         <v>0.6875</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E47" t="s">
         <v>65</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F47" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add recording links to schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenfra/NBISCourses/scRNAseq/workshop-scRNAseq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFADA04-2E23-3B44-B077-F414B0FC4A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A131CE26-ACD8-8E47-BA54-BDA7C998D97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18160" yWindow="3220" windowWidth="28620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1420" yWindow="1440" windowWidth="35000" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="91">
   <si>
     <t>date</t>
   </si>
@@ -268,6 +268,39 @@
   </si>
   <si>
     <t>lectures/BYOD_intro.pdf</t>
+  </si>
+  <si>
+    <t>https://youtu.be/OccS8ZFN0E4</t>
+  </si>
+  <si>
+    <t>https://youtu.be/gAAs4BWfAtM</t>
+  </si>
+  <si>
+    <t>https://youtu.be/23C5LFXZZ2U</t>
+  </si>
+  <si>
+    <t>https://youtu.be/X6zQ0a0da8I</t>
+  </si>
+  <si>
+    <t>https://youtu.be/a-vzYSYA9mg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/7D6iMgvPFZk</t>
+  </si>
+  <si>
+    <t>https://youtu.be/FvIsISt8Auw</t>
+  </si>
+  <si>
+    <t>https://youtu.be/-DnF0uD3euo</t>
+  </si>
+  <si>
+    <t>https://youtu.be/lGAcQqeEOzA</t>
+  </si>
+  <si>
+    <t>https://youtu.be/h8XZzdBMokc</t>
+  </si>
+  <si>
+    <t>https://youtu.be/epN5KSt6qZg</t>
   </si>
 </sst>
 </file>
@@ -312,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -321,6 +354,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -408,9 +442,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -448,7 +482,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -554,7 +588,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -696,7 +730,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -706,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -803,7 +837,9 @@
       <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C4" s="2">
@@ -832,6 +868,9 @@
       <c r="H5" t="s">
         <v>16</v>
       </c>
+      <c r="K5" s="4" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C6" s="2">
@@ -906,6 +945,9 @@
       <c r="H10" t="s">
         <v>26</v>
       </c>
+      <c r="K10" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C11" s="2">
@@ -943,7 +985,9 @@
       <c r="H12" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="3"/>
+      <c r="K12" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C13" s="2">
@@ -1001,7 +1045,9 @@
       <c r="H16" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="3"/>
+      <c r="K16" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C17" s="2">
@@ -1048,6 +1094,9 @@
       <c r="H19" t="s">
         <v>36</v>
       </c>
+      <c r="K19" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C20" s="2">
@@ -1121,7 +1170,9 @@
       <c r="I24" t="s">
         <v>75</v>
       </c>
-      <c r="K24" s="3"/>
+      <c r="K24" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C25" s="2">
@@ -1142,7 +1193,9 @@
       <c r="I25" t="s">
         <v>76</v>
       </c>
-      <c r="K25" s="3"/>
+      <c r="K25" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C26" s="2">
@@ -1172,6 +1225,9 @@
       <c r="H27" t="s">
         <v>40</v>
       </c>
+      <c r="K27" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C28" s="2">
@@ -1255,7 +1311,9 @@
       <c r="H32" t="s">
         <v>46</v>
       </c>
-      <c r="K32" s="3"/>
+      <c r="K32" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C33" s="2">
@@ -1312,6 +1370,9 @@
       </c>
       <c r="H36" t="s">
         <v>50</v>
+      </c>
+      <c r="K36" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -1486,6 +1547,7 @@
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="J39" r:id="rId2" xr:uid="{02E4C23A-A3EF-964B-8695-A052AA7101DD}"/>
+    <hyperlink ref="K5" r:id="rId3" xr:uid="{9D7E1F62-7D51-AC46-A470-603E03028633}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>